<commit_message>
Parallelized loops no large files
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{82A791FC-64D1-2346-A7BA-94034F67C07C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D9FF68C-C846-9D47-A419-9BA02FC20DFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2540" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>tau = 0.6</t>
   </si>
@@ -48,18 +48,6 @@
     <t>Tlin</t>
   </si>
   <si>
-    <t>80x80</t>
-  </si>
-  <si>
-    <t>120x120</t>
-  </si>
-  <si>
-    <t>160x160</t>
-  </si>
-  <si>
-    <t>200x200</t>
-  </si>
-  <si>
     <t>Hsou</t>
   </si>
   <si>
@@ -79,6 +67,21 @@
   </si>
   <si>
     <t>Gallium</t>
+  </si>
+  <si>
+    <t>Ra=10^8</t>
+  </si>
+  <si>
+    <t>140x140</t>
+  </si>
+  <si>
+    <t>180x180</t>
+  </si>
+  <si>
+    <t>225x225</t>
+  </si>
+  <si>
+    <t>100x100</t>
   </si>
 </sst>
 </file>
@@ -448,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F026E8-BD5F-7A4F-841B-25764A0F874E}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -462,15 +465,15 @@
   <sheetData>
     <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -490,12 +493,12 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>3</v>
@@ -503,7 +506,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
@@ -511,7 +514,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
@@ -519,7 +522,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
@@ -527,44 +530,44 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" t="s">
         <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="D13" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C14" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="D14" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C16" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D16" t="s">
         <v>3</v>
@@ -572,10 +575,26 @@
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>8</v>
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>11</v>
+      </c>
+      <c r="D18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
freeze plug ss works but unstable
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A6091B8-750E-5941-9939-05D6D998DFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B32B1CF-FE90-0849-B4FC-5B2776E51672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
@@ -144,7 +144,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -154,6 +154,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -170,13 +176,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -494,7 +501,7 @@
   <dimension ref="A1:G28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -573,6 +580,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
       <c r="C11" t="s">
         <v>19</v>
       </c>
@@ -608,6 +616,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
       <c r="C15" t="s">
         <v>19</v>
       </c>

</xml_diff>

<commit_message>
1D Stefan codes updated
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B32B1CF-FE90-0849-B4FC-5B2776E51672}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2C4BEF-21E4-1D46-B174-0AD70FA43CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
   <si>
     <t>tau = 0.6</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Octadecane</t>
   </si>
   <si>
-    <t>Gallium</t>
-  </si>
-  <si>
     <t>Ra=10^8</t>
   </si>
   <si>
@@ -106,6 +103,39 @@
   </si>
   <si>
     <t>Meltfront for diff. Mesh</t>
+  </si>
+  <si>
+    <t>Freeze plug</t>
+  </si>
+  <si>
+    <t>Degrees</t>
+  </si>
+  <si>
+    <t>Wall width</t>
+  </si>
+  <si>
+    <t>Freezing</t>
+  </si>
+  <si>
+    <t>Melting</t>
+  </si>
+  <si>
+    <t>High res</t>
+  </si>
+  <si>
+    <t>Natural convection</t>
+  </si>
+  <si>
+    <t>Stefan</t>
+  </si>
+  <si>
+    <t>Benchmark with Shafer</t>
+  </si>
+  <si>
+    <t>10 cm, 5 K</t>
+  </si>
+  <si>
+    <t>DT</t>
   </si>
 </sst>
 </file>
@@ -144,7 +174,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -163,6 +193,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -176,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -184,6 +220,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -498,138 +537,259 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F026E8-BD5F-7A4F-841B-25764A0F874E}">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="5.5" customWidth="1"/>
+    <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+      <c r="M1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H3" s="8"/>
+      <c r="I3" s="8"/>
+      <c r="K3" s="8"/>
+      <c r="L3" s="8"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H4">
+        <v>30</v>
+      </c>
+      <c r="I4">
+        <v>2.5</v>
+      </c>
+      <c r="J4">
+        <v>40</v>
+      </c>
+      <c r="K4" s="8"/>
+      <c r="L4" s="7"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>80</v>
+      </c>
+      <c r="K5" s="6"/>
+      <c r="L5" s="7"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="7"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I6">
+        <v>5</v>
+      </c>
+      <c r="J6">
+        <v>40</v>
+      </c>
+      <c r="K6" s="8"/>
+      <c r="L6" s="7"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>80</v>
+      </c>
+      <c r="K7" s="7"/>
+      <c r="L7" s="7"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H8">
+        <v>60</v>
+      </c>
+      <c r="I8">
+        <v>2.5</v>
+      </c>
+      <c r="J8">
+        <v>40</v>
+      </c>
+      <c r="K8" s="8"/>
+      <c r="L8" s="7"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>80</v>
+      </c>
+      <c r="K9" s="7"/>
+      <c r="L9" s="7"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I10">
+        <v>5</v>
+      </c>
+      <c r="J10">
+        <v>40</v>
+      </c>
+      <c r="K10" s="8"/>
+      <c r="L10" s="7"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B11" s="6"/>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D11" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>80</v>
+      </c>
+      <c r="K11" s="7"/>
+      <c r="L11" s="7"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H12">
+        <v>90</v>
+      </c>
+      <c r="I12">
+        <v>2.5</v>
+      </c>
+      <c r="J12">
+        <v>40</v>
+      </c>
+      <c r="K12" s="8"/>
+      <c r="L12" s="7"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>80</v>
+      </c>
+      <c r="K13" s="7"/>
+      <c r="L13" s="7"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H14" s="8"/>
+      <c r="I14">
+        <v>5</v>
+      </c>
+      <c r="J14">
+        <v>40</v>
+      </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="7"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B15" s="6"/>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="H15" s="8"/>
+      <c r="I15" s="8"/>
+      <c r="J15">
+        <v>80</v>
+      </c>
+      <c r="K15" s="7"/>
+      <c r="L15" s="7"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C17" t="s">
         <v>8</v>
       </c>
@@ -637,7 +797,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C18" t="s">
         <v>8</v>
       </c>
@@ -645,68 +805,89 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C19" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C20" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" s="9"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C24" t="s">
         <v>15</v>
       </c>
-      <c r="C23" t="s">
+      <c r="E24" t="s">
         <v>16</v>
       </c>
-      <c r="E23" t="s">
+      <c r="L24" t="s">
+        <v>31</v>
+      </c>
+      <c r="N24" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C25" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C24" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C25" t="s">
-        <v>20</v>
       </c>
       <c r="E25" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C26" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C27" t="s">
+        <v>22</v>
+      </c>
+      <c r="E27" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C27" t="s">
-        <v>23</v>
-      </c>
-      <c r="E27" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C28" t="s">
         <v>22</v>
+      </c>
+      <c r="E28" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C29" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Multiple small changes 2
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB2C4BEF-21E4-1D46-B174-0AD70FA43CB1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD58F22-0A2B-D04D-A838-8D907395417A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
+    <workbookView xWindow="80" yWindow="-21980" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
   <dimension ref="A1:N29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M11" sqref="M11"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -622,10 +622,10 @@
       <c r="J5">
         <v>80</v>
       </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="7"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="7"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
@@ -682,7 +682,7 @@
       <c r="J9">
         <v>80</v>
       </c>
-      <c r="K9" s="7"/>
+      <c r="K9" s="4"/>
       <c r="L9" s="7"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.2">
@@ -703,7 +703,7 @@
       <c r="L10" s="7"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B11" s="6"/>
+      <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>18</v>
       </c>
@@ -713,7 +713,7 @@
       <c r="J11">
         <v>80</v>
       </c>
-      <c r="K11" s="7"/>
+      <c r="K11" s="6"/>
       <c r="L11" s="7"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.2">
@@ -769,7 +769,7 @@
       <c r="L14" s="7"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.2">
-      <c r="B15" s="6"/>
+      <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
Multiple small changes 3
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCD58F22-0A2B-D04D-A838-8D907395417A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E8904B-B3AA-F345-83AF-427F2B20EBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="80" yWindow="-21980" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="35">
   <si>
     <t>tau = 0.6</t>
   </si>
@@ -136,13 +136,16 @@
   </si>
   <si>
     <t>DT</t>
+  </si>
+  <si>
+    <t>Low res</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -169,6 +172,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -212,17 +222,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9F026E8-BD5F-7A4F-841B-25764A0F874E}">
-  <dimension ref="A1:N29"/>
+  <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -550,7 +561,7 @@
     <col min="7" max="7" width="12.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>9</v>
       </c>
@@ -560,8 +571,11 @@
       <c r="M1" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
@@ -586,24 +600,30 @@
       <c r="N2" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="O2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="H3" s="8"/>
-      <c r="I3" s="8"/>
-      <c r="K3" s="8"/>
-      <c r="L3" s="8"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="K3" s="7"/>
+      <c r="L3" s="7"/>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B4" s="3"/>
       <c r="C4" t="s">
         <v>1</v>
       </c>
       <c r="H4">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="I4">
         <v>2.5</v>
@@ -611,10 +631,10 @@
       <c r="J4">
         <v>40</v>
       </c>
-      <c r="K4" s="8"/>
-      <c r="L4" s="7"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K4" s="7"/>
+      <c r="L4" s="6"/>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
       <c r="C5" t="s">
         <v>2</v>
@@ -625,9 +645,11 @@
       <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
-      <c r="N5" s="6"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="N5" s="5"/>
+      <c r="O5" s="4"/>
+      <c r="P5" s="10"/>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
       <c r="C6" t="s">
         <v>20</v>
@@ -638,20 +660,20 @@
       <c r="J6">
         <v>40</v>
       </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="7"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K6" s="7"/>
+      <c r="L6" s="6"/>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
         <v>6</v>
       </c>
       <c r="J7">
         <v>80</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="7"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K7" s="9"/>
+      <c r="L7" s="6"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
       <c r="C8" t="s">
         <v>12</v>
@@ -668,10 +690,10 @@
       <c r="J8">
         <v>40</v>
       </c>
-      <c r="K8" s="8"/>
-      <c r="L8" s="7"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K8" s="7"/>
+      <c r="L8" s="6"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
       <c r="C9" t="s">
         <v>11</v>
@@ -683,9 +705,13 @@
         <v>80</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="7"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="L9" s="6"/>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="4"/>
       <c r="C10" t="s">
         <v>13</v>
@@ -699,10 +725,14 @@
       <c r="J10">
         <v>40</v>
       </c>
-      <c r="K10" s="8"/>
-      <c r="L10" s="7"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="4"/>
       <c r="C11" t="s">
         <v>18</v>
@@ -713,10 +743,10 @@
       <c r="J11">
         <v>80</v>
       </c>
-      <c r="K11" s="6"/>
-      <c r="L11" s="7"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K11" s="4"/>
+      <c r="L11" s="6"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
       <c r="C12" t="s">
         <v>12</v>
@@ -733,10 +763,10 @@
       <c r="J12">
         <v>40</v>
       </c>
-      <c r="K12" s="8"/>
-      <c r="L12" s="7"/>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K12" s="7"/>
+      <c r="L12" s="6"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="5"/>
       <c r="C13" t="s">
         <v>11</v>
@@ -747,10 +777,10 @@
       <c r="J13">
         <v>80</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="7"/>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K13" s="4"/>
+      <c r="L13" s="6"/>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="5"/>
       <c r="C14" t="s">
         <v>13</v>
@@ -758,17 +788,17 @@
       <c r="D14" t="s">
         <v>4</v>
       </c>
-      <c r="H14" s="8"/>
+      <c r="H14" s="7"/>
       <c r="I14">
         <v>5</v>
       </c>
       <c r="J14">
         <v>40</v>
       </c>
-      <c r="K14" s="8"/>
-      <c r="L14" s="7"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K14" s="7"/>
+      <c r="L14" s="6"/>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B15" s="4"/>
       <c r="C15" t="s">
         <v>18</v>
@@ -776,15 +806,15 @@
       <c r="D15" t="s">
         <v>4</v>
       </c>
-      <c r="H15" s="8"/>
-      <c r="I15" s="8"/>
+      <c r="H15" s="7"/>
+      <c r="I15" s="7"/>
       <c r="J15">
         <v>80</v>
       </c>
-      <c r="K15" s="7"/>
-      <c r="L15" s="7"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="K15" s="9"/>
+      <c r="L15" s="6"/>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>7</v>
       </c>
@@ -837,7 +867,7 @@
       <c r="L23" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="N23" s="9"/>
+      <c r="N23" s="8"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="C24" t="s">

</xml_diff>

<commit_message>
Added comments to Hsou and streaming funcs
</commit_message>
<xml_diff>
--- a/Working code/To-do simulations.xlsx
+++ b/Working code/To-do simulations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jesper/Documents/MEP/Code/Working code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E8904B-B3AA-F345-83AF-427F2B20EBC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C64D8C69-9702-D246-97E8-ECFA748F0BB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
+    <workbookView xWindow="0" yWindow="3000" windowWidth="28800" windowHeight="18000" xr2:uid="{0108CE3A-3B0D-0D44-A64A-4D361F588922}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -232,8 +232,8 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +551,7 @@
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N16" sqref="N16"/>
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -632,7 +632,7 @@
         <v>40</v>
       </c>
       <c r="K4" s="7"/>
-      <c r="L4" s="6"/>
+      <c r="L4" s="4"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B5" s="3"/>
@@ -647,7 +647,7 @@
       <c r="M5" s="4"/>
       <c r="N5" s="5"/>
       <c r="O5" s="4"/>
-      <c r="P5" s="10"/>
+      <c r="P5" s="9"/>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B6" s="4"/>
@@ -661,7 +661,7 @@
         <v>40</v>
       </c>
       <c r="K6" s="7"/>
-      <c r="L6" s="6"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
@@ -670,8 +670,8 @@
       <c r="J7">
         <v>80</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="6"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="7"/>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="4"/>
@@ -691,7 +691,7 @@
         <v>40</v>
       </c>
       <c r="K8" s="7"/>
-      <c r="L8" s="6"/>
+      <c r="L8" s="4"/>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B9" s="4"/>
@@ -705,7 +705,7 @@
         <v>80</v>
       </c>
       <c r="K9" s="4"/>
-      <c r="L9" s="6"/>
+      <c r="L9" s="4"/>
       <c r="M9" s="7"/>
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
@@ -726,7 +726,7 @@
         <v>40</v>
       </c>
       <c r="K10" s="7"/>
-      <c r="L10" s="6"/>
+      <c r="L10" s="10"/>
       <c r="M10" s="7"/>
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
@@ -744,7 +744,7 @@
         <v>80</v>
       </c>
       <c r="K11" s="4"/>
-      <c r="L11" s="6"/>
+      <c r="L11" s="4"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="5"/>
@@ -811,7 +811,7 @@
       <c r="J15">
         <v>80</v>
       </c>
-      <c r="K15" s="9"/>
+      <c r="K15" s="4"/>
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.2">

</xml_diff>